<commit_message>
Add RF range test data and update data sheet
</commit_message>
<xml_diff>
--- a/hardware/ZRADBOM.xlsx
+++ b/hardware/ZRADBOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Documents\GitHub\ZReach\hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Documents\GitHub\ZRAD\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA6C627-5261-47E6-993B-0DBC4C69C19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9238A82-5D06-4CA0-9421-D6B415FB43AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3885" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -74,36 +74,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{3F069F16-5293-42E4-9762-AFE6A20DCBF4}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>eric:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-5 As and 10 Bs</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="199">
   <si>
     <t>Item #</t>
   </si>
@@ -189,9 +165,6 @@
     <t>Or other material, roughly 28"x12"</t>
   </si>
   <si>
-    <t>Bill of material for the Z-Wave Alliance Z-Reach Reference Controller.</t>
-  </si>
-  <si>
     <t>Initial file creation</t>
   </si>
   <si>
@@ -631,6 +604,78 @@
   </si>
   <si>
     <t>336-5888-1-ND‎</t>
+  </si>
+  <si>
+    <t>OSHPark.com</t>
+  </si>
+  <si>
+    <t>Bare PCB</t>
+  </si>
+  <si>
+    <t>Cost estimate is assuming panelized PCB</t>
+  </si>
+  <si>
+    <t>Antenna</t>
+  </si>
+  <si>
+    <t>Enclosure</t>
+  </si>
+  <si>
+    <t>USB Cable</t>
+  </si>
+  <si>
+    <t>JCG402LR-2</t>
+  </si>
+  <si>
+    <t>MISC</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Low cost recommended antenna - there are several more expensive ones</t>
+  </si>
+  <si>
+    <t>Expensive but prevents reverse battery insertion which is not protected by circuitry</t>
+  </si>
+  <si>
+    <t>ED=End Device vs. Controller</t>
+  </si>
+  <si>
+    <t>ED does not need USB or LDO</t>
+  </si>
+  <si>
+    <t>TOTAL COST:</t>
+  </si>
+  <si>
+    <t>Your cost could be significantly lower depending on volume</t>
+  </si>
+  <si>
+    <t>Packaging</t>
+  </si>
+  <si>
+    <t>Total cost is for a controller @1K qty with distributor pricing from Digikey</t>
+  </si>
+  <si>
+    <t>Component cost ONLY and does not include assembly, testing or packaging</t>
+  </si>
+  <si>
+    <t>Updated with more details and cost analysis</t>
+  </si>
+  <si>
+    <t>Bill of material for the Z-Wave Alliance Reference Application Design (ZRAD)</t>
+  </si>
+  <si>
+    <t>The Test Jig is used to program and test assembled ZRAD boards.</t>
+  </si>
+  <si>
+    <t>This is a work-in-progress and has not yet been stated in April 2024</t>
   </si>
 </sst>
 </file>
@@ -641,7 +686,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -711,6 +756,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -720,7 +780,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -890,13 +950,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -949,6 +1022,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -966,6 +1050,946 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18317054469314931"/>
+          <c:y val="0.16315377534848599"/>
+          <c:w val="0.69358400424666022"/>
+          <c:h val="0.70446752790838318"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'BOM Controller'!$S$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'BOM Controller'!$R$5:$R$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Z-Wave MCU/Radio</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>USB2.0 UART</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Antenna</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bare PCB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SMA Verticle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MISC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'BOM Controller'!$S$5:$S$10</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.8499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7059999999999977</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B7CA-4CA6-B883-B6FA7044AF28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>204786</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC10EF3-925A-24BB-02D0-A043D5C4F2DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1234,7 +2258,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,7 +2268,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
-        <v>28</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1262,11 +2286,16 @@
         <v>45338</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="4">
+        <v>45406</v>
+      </c>
+      <c r="B11" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -1287,11 +2316,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomLeft" activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,7 +2336,7 @@
     <col min="9" max="9" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1342,13 +2371,13 @@
         <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -1362,7 +2391,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>18</v>
@@ -1378,38 +2407,35 @@
         <v>4.8499999999999996</v>
       </c>
       <c r="J2" s="10">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K2" s="13">
         <f>$M$2*G2-J2</f>
         <v>0</v>
       </c>
-      <c r="M2">
-        <v>15</v>
-      </c>
       <c r="N2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="22">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G3" s="11">
         <v>1</v>
@@ -1418,7 +2444,7 @@
         <v>2.34</v>
       </c>
       <c r="I3" s="12">
-        <f t="shared" ref="I3:I34" si="0">H3*G3</f>
+        <f t="shared" ref="I3:I36" si="0">H3*G3</f>
         <v>2.34</v>
       </c>
       <c r="J3" s="10">
@@ -1426,28 +2452,28 @@
       </c>
       <c r="K3" s="13">
         <f t="shared" ref="K3:K34" si="1">$M$2*G3-J3</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="22">
         <f t="shared" ref="A4:A42" si="2">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="11">
         <v>1</v>
@@ -1464,28 +2490,34 @@
       </c>
       <c r="K4" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>184</v>
+      </c>
+      <c r="S4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B5" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="26" t="s">
         <v>41</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>42</v>
       </c>
       <c r="G5" s="11">
         <v>1</v>
@@ -1502,28 +2534,39 @@
       </c>
       <c r="K5" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>188</v>
+      </c>
+      <c r="R5" t="str">
+        <f>$D$2</f>
+        <v>Z-Wave MCU/Radio</v>
+      </c>
+      <c r="S5" s="2">
+        <f>I2</f>
+        <v>4.8499999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>47</v>
       </c>
       <c r="G6" s="11">
         <v>3</v>
@@ -1540,28 +2583,39 @@
       </c>
       <c r="K6" s="13">
         <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>189</v>
+      </c>
+      <c r="R6" t="str">
+        <f>$D$3</f>
+        <v>USB2.0 UART</v>
+      </c>
+      <c r="S6" s="2">
+        <f>I3</f>
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="22">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B7" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>49</v>
       </c>
       <c r="G7" s="11">
         <v>3</v>
@@ -1578,28 +2632,36 @@
       </c>
       <c r="K7" s="13">
         <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R7" t="str">
+        <f>$D$36</f>
+        <v>Antenna</v>
+      </c>
+      <c r="S7" s="2">
+        <f>I36</f>
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="22">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B8" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" s="29" t="s">
         <v>52</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>53</v>
       </c>
       <c r="G8" s="11">
         <v>1</v>
@@ -1616,28 +2678,36 @@
       </c>
       <c r="K8" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R8" t="str">
+        <f>$D$35</f>
+        <v>Bare PCB</v>
+      </c>
+      <c r="S8" s="2">
+        <f>I35</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B9" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="G9" s="11">
         <v>1</v>
@@ -1654,28 +2724,36 @@
       </c>
       <c r="K9" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R9" t="str">
+        <f>$D$17</f>
+        <v>SMA Verticle</v>
+      </c>
+      <c r="S9" s="2">
+        <f>I17</f>
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="22">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="B10" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>60</v>
       </c>
       <c r="G10" s="11">
         <v>1</v>
@@ -1692,28 +2770,35 @@
       </c>
       <c r="K10" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R10" t="s">
+        <v>182</v>
+      </c>
+      <c r="S10" s="2">
+        <f>I40-SUM(S5:S9)</f>
+        <v>2.7059999999999977</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="B11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>62</v>
-      </c>
       <c r="E11" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="11">
         <v>1</v>
@@ -1730,28 +2815,35 @@
       </c>
       <c r="K11" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R11" t="s">
+        <v>185</v>
+      </c>
+      <c r="S11" s="2">
+        <f>SUM(S5:S10)</f>
+        <v>14.655999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="B12" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G12" s="11">
         <v>4</v>
@@ -1768,28 +2860,28 @@
       </c>
       <c r="K12" s="13">
         <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="B13" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>70</v>
       </c>
       <c r="G13" s="11">
         <v>3</v>
@@ -1806,28 +2898,28 @@
       </c>
       <c r="K13" s="13">
         <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="D14" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="31" t="s">
-        <v>74</v>
-      </c>
       <c r="E14" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G14" s="11">
         <v>1</v>
@@ -1844,28 +2936,28 @@
       </c>
       <c r="K14" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>78</v>
-      </c>
       <c r="E15" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G15" s="11">
         <v>1</v>
@@ -1882,31 +2974,31 @@
       </c>
       <c r="K15" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="22">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G16" s="11">
         <v>1</v>
@@ -1923,7 +3015,7 @@
       </c>
       <c r="K16" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1932,19 +3024,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>88</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>89</v>
       </c>
       <c r="G17" s="11">
         <v>1</v>
@@ -1961,7 +3053,7 @@
       </c>
       <c r="K17" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1970,39 +3062,39 @@
         <v>17</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="D18" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>93</v>
-      </c>
       <c r="G18" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="12">
         <v>0.31</v>
       </c>
       <c r="I18" s="12">
         <f t="shared" si="0"/>
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="J18" s="10">
         <v>0</v>
       </c>
       <c r="K18" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2011,19 +3103,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="E19" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>97</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>98</v>
       </c>
       <c r="G19" s="11">
         <v>1</v>
@@ -2040,7 +3132,7 @@
       </c>
       <c r="K19" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2049,19 +3141,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>100</v>
-      </c>
       <c r="E20" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G20" s="11">
         <v>1</v>
@@ -2078,7 +3170,7 @@
       </c>
       <c r="K20" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -2087,19 +3179,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G21" s="11">
         <v>1</v>
@@ -2116,7 +3208,7 @@
       </c>
       <c r="K21" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2125,19 +3217,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G22" s="11">
         <v>1</v>
@@ -2154,7 +3246,7 @@
       </c>
       <c r="K22" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2163,19 +3255,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="E23" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>113</v>
       </c>
       <c r="G23" s="11">
         <v>1</v>
@@ -2192,7 +3284,7 @@
       </c>
       <c r="K23" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2201,19 +3293,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="E24" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>115</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>116</v>
       </c>
       <c r="G24" s="11">
         <v>3</v>
@@ -2230,7 +3322,7 @@
       </c>
       <c r="K24" s="13">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2239,19 +3331,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="E25" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>119</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>120</v>
       </c>
       <c r="G25" s="11">
         <v>2</v>
@@ -2268,7 +3360,7 @@
       </c>
       <c r="K25" s="13">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2277,19 +3369,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="E26" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>122</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>123</v>
       </c>
       <c r="G26" s="11">
         <v>2</v>
@@ -2306,7 +3398,7 @@
       </c>
       <c r="K26" s="13">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2315,19 +3407,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" s="10" t="s">
+      <c r="E27" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="G27" s="11">
         <v>1</v>
@@ -2344,7 +3436,7 @@
       </c>
       <c r="K27" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2353,19 +3445,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="F28" s="10" t="s">
         <v>129</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>130</v>
       </c>
       <c r="G28" s="11">
         <v>1</v>
@@ -2382,7 +3474,7 @@
       </c>
       <c r="K28" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2391,19 +3483,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>132</v>
-      </c>
       <c r="E29" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G29" s="11">
         <v>1</v>
@@ -2420,7 +3512,7 @@
       </c>
       <c r="K29" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2429,19 +3521,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F30" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="G30" s="11">
         <v>2</v>
@@ -2458,7 +3550,7 @@
       </c>
       <c r="K30" s="13">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2467,19 +3559,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="10" t="s">
+      <c r="E31" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="F31" s="10" t="s">
         <v>139</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>140</v>
       </c>
       <c r="G31" s="11">
         <v>1</v>
@@ -2496,7 +3588,7 @@
       </c>
       <c r="K31" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2505,19 +3597,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="F32" s="10" t="s">
         <v>144</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>145</v>
       </c>
       <c r="G32" s="11">
         <v>1</v>
@@ -2534,10 +3626,10 @@
       </c>
       <c r="K32" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -2546,39 +3638,39 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="D33" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>149</v>
-      </c>
       <c r="E33" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G33" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" s="12">
         <v>0.2</v>
       </c>
       <c r="I33" s="12">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="J33" s="10">
         <v>0</v>
       </c>
       <c r="K33" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2587,36 +3679,39 @@
         <v>33</v>
       </c>
       <c r="B34" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="F34" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="F34" s="10" t="s">
-        <v>157</v>
-      </c>
       <c r="G34" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" s="12">
         <v>2.5099999999999998</v>
       </c>
       <c r="I34" s="12">
         <f t="shared" si="0"/>
-        <v>2.5099999999999998</v>
+        <v>0</v>
       </c>
       <c r="J34" s="10">
         <v>0</v>
       </c>
       <c r="K34" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="M34" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2624,32 +3719,62 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="B35" s="10"/>
+      <c r="B35" s="10" t="s">
+        <v>175</v>
+      </c>
       <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="D35" s="10" t="s">
+        <v>176</v>
+      </c>
       <c r="E35" s="15"/>
       <c r="F35" s="10"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
+      <c r="G35" s="11">
+        <v>1</v>
+      </c>
+      <c r="H35" s="12">
+        <v>1</v>
+      </c>
+      <c r="I35" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J35" s="10"/>
       <c r="K35" s="13"/>
+      <c r="M35" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="B36" s="10"/>
+      <c r="B36" t="s">
+        <v>181</v>
+      </c>
       <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
+      <c r="D36" s="10" t="s">
+        <v>178</v>
+      </c>
       <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
+      <c r="F36" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="G36" s="11">
+        <v>1</v>
+      </c>
+      <c r="H36" s="12">
+        <v>2.54</v>
+      </c>
+      <c r="I36" s="12">
+        <f t="shared" si="0"/>
+        <v>2.54</v>
+      </c>
       <c r="J36" s="10"/>
       <c r="K36" s="13"/>
+      <c r="M36" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
@@ -2658,7 +3783,9 @@
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
+      <c r="D37" s="10" t="s">
+        <v>179</v>
+      </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="11"/>
@@ -2674,7 +3801,9 @@
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
+      <c r="D38" s="10" t="s">
+        <v>180</v>
+      </c>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
       <c r="G38" s="11"/>
@@ -2690,16 +3819,18 @@
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
+      <c r="D39" s="10" t="s">
+        <v>192</v>
+      </c>
       <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
       <c r="J39" s="10"/>
       <c r="K39" s="13"/>
     </row>
-    <row r="40" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -2708,12 +3839,20 @@
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
+      <c r="F40" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="G40" s="39"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="35">
+        <f>SUM(I2:I39)</f>
+        <v>14.655999999999999</v>
+      </c>
       <c r="J40" s="10"/>
       <c r="K40" s="13"/>
+      <c r="M40" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
@@ -2730,6 +3869,9 @@
       <c r="I41" s="12"/>
       <c r="J41" s="10"/>
       <c r="K41" s="13"/>
+      <c r="M41" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
@@ -2746,6 +3888,9 @@
       <c r="I42" s="19"/>
       <c r="J42" s="17"/>
       <c r="K42" s="20"/>
+      <c r="M42" t="s">
+        <v>194</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2760,19 +3905,21 @@
     <hyperlink ref="B11" r:id="rId9" display="https://www.digikey.com/en/products/detail/murata-electronics/GJM1555C1H1R3BB01D/2592879" xr:uid="{744A2046-458B-4F89-A568-71EDB3430337}"/>
     <hyperlink ref="B12" r:id="rId10" display="https://www.digikey.com/en/products/detail/murata-electronics/GRM21BR71C475KE51L/6606095" xr:uid="{D1C9B504-EA11-47B0-A380-66685325C2A3}"/>
     <hyperlink ref="B13" r:id="rId11" display="https://www.digikey.com/en/products/detail/murata-electronics/GCM188L81H104KA57D/2591908" xr:uid="{CF280619-1A25-4425-9524-CC71C1A3F4D8}"/>
+    <hyperlink ref="F36" r:id="rId12" display="https://www.digikey.com/en/products/detail/jc-antenna/JCG402LR-2/15814458" xr:uid="{C038367E-887A-4E6B-BA17-618664AFA725}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="92" orientation="portrait" r:id="rId12"/>
-  <legacyDrawing r:id="rId13"/>
+  <pageSetup scale="92" orientation="portrait" r:id="rId13"/>
+  <drawing r:id="rId14"/>
+  <legacyDrawing r:id="rId15"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30C90F15-B4E9-4E34-8D0E-C7A19BDCE1DA}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2967,6 +4114,16 @@
         <v>14</v>
       </c>
     </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>198</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{1FDC4E02-AAB4-4DDC-98A7-899E4AA5F8EF}"/>

</xml_diff>